<commit_message>
update to ui and layout
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Arbeit/12-TUM/Repos_Misc/Draw_my_timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF46C88-DB3D-FA4C-AB0F-C148D4B24368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E481DE9-3200-604D-8784-241B8AF246D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="780" windowWidth="39700" windowHeight="25800" xr2:uid="{A549E01A-21D3-B048-ACE5-6C86109A1619}"/>
+    <workbookView xWindow="1420" yWindow="780" windowWidth="39700" windowHeight="25800" activeTab="4" xr2:uid="{A549E01A-21D3-B048-ACE5-6C86109A1619}"/>
   </bookViews>
   <sheets>
-    <sheet name="Learning_room" sheetId="2" r:id="rId1"/>
-    <sheet name="Carpentry_workshop" sheetId="5" r:id="rId2"/>
-    <sheet name="Office" sheetId="8" r:id="rId3"/>
-    <sheet name="Emergeny_room" sheetId="6" r:id="rId4"/>
-    <sheet name="Industrial_production_line" sheetId="7" r:id="rId5"/>
+    <sheet name="Example_1" sheetId="2" r:id="rId1"/>
+    <sheet name="Example_2" sheetId="5" r:id="rId2"/>
+    <sheet name="Example_3" sheetId="8" r:id="rId3"/>
+    <sheet name="Example_4" sheetId="6" r:id="rId4"/>
+    <sheet name="Example_5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -247,6 +247,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -257,15 +266,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -604,35 +604,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098B3F44-401D-744B-84F3-972014BD43E0}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" workbookViewId="0">
+    <sheetView zoomScale="220" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -708,28 +708,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -788,182 +788,182 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="12">
         <v>0.25</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13">
         <v>656</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="12">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13">
         <v>656</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13">
         <v>656</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="12">
         <v>0.375</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13">
         <v>656</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13">
         <v>656</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="12">
         <v>0.625</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="13">
         <v>656</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13">
         <v>656</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="11">
         <v>3</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13">
         <v>656</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="11">
         <v>2</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="12">
         <v>0.75</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <v>656</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="11">
         <v>8</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="12">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="12">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="13">
         <v>656</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -990,28 +990,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1080,35 +1080,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8806D41-084C-E14B-9A89-5BDC6021F2D3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1223,12 +1223,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e7f6b4e8-9e4f-40ca-b4d8-5afb38350410" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f2f12b5a-3239-485c-afa7-8bfa8665860f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1433,20 +1435,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e7f6b4e8-9e4f-40ca-b4d8-5afb38350410" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f2f12b5a-3239-485c-afa7-8bfa8665860f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A32B19E-66BB-48BF-8400-E4A784426B82}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A27E043-F4E1-471F-980E-39AA631A596B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e7f6b4e8-9e4f-40ca-b4d8-5afb38350410"/>
+    <ds:schemaRef ds:uri="f2f12b5a-3239-485c-afa7-8bfa8665860f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1471,18 +1480,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A27E043-F4E1-471F-980E-39AA631A596B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A32B19E-66BB-48BF-8400-E4A784426B82}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e7f6b4e8-9e4f-40ca-b4d8-5afb38350410"/>
-    <ds:schemaRef ds:uri="f2f12b5a-3239-485c-afa7-8bfa8665860f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>